<commit_message>
Fix for pirate faction not triggering scaling
Script Scaling isn't 100% reliable seems quest zones do something different. The perk method might be better.
</commit_message>
<xml_diff>
--- a/NPCScaling.xlsx
+++ b/NPCScaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Public\Starfield Mods\starfield-level-based-scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39437D7B-E723-48D4-B702-0B3CD765A56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB60762-120A-4479-A924-A87BCEA8691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
+    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
   </bookViews>
   <sheets>
     <sheet name="Spacers (Full DS)" sheetId="15" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="321">
   <si>
     <t>Level</t>
   </si>
@@ -298,9 +298,6 @@
     <t>EncCrimsonFleet05</t>
   </si>
   <si>
-    <t>Pirate</t>
-  </si>
-  <si>
     <t>Pirate Brigand</t>
   </si>
   <si>
@@ -355,12 +352,6 @@
     <t>Pirate Legend</t>
   </si>
   <si>
-    <t>Pirate Peon</t>
-  </si>
-  <si>
-    <t>Pirate Ransacker</t>
-  </si>
-  <si>
     <t>Syndicate Launderer</t>
   </si>
   <si>
@@ -640,45 +631,6 @@
     <t>Max Level</t>
   </si>
   <si>
-    <t>DSPiratePeon</t>
-  </si>
-  <si>
-    <t>DSPirateBrigand</t>
-  </si>
-  <si>
-    <t>DSPirateFreebooter</t>
-  </si>
-  <si>
-    <t>DSPirateRover</t>
-  </si>
-  <si>
-    <t>DSPirateMarauder</t>
-  </si>
-  <si>
-    <t>DSPirateRansacker</t>
-  </si>
-  <si>
-    <t>DSPirateCorsair</t>
-  </si>
-  <si>
-    <t>DSPiratePlunderer</t>
-  </si>
-  <si>
-    <t>DSPirateReaver</t>
-  </si>
-  <si>
-    <t>DSPirateCutthroat</t>
-  </si>
-  <si>
-    <t>DSPirateFlayer</t>
-  </si>
-  <si>
-    <t>DSPirateCaptain</t>
-  </si>
-  <si>
-    <t>DSPirateLegend</t>
-  </si>
-  <si>
     <t>Level Mult</t>
   </si>
   <si>
@@ -1016,6 +968,45 @@
   </si>
   <si>
     <t>LLI_Ecliptic_Heavy_Boss [LVLI:0025C5E7]</t>
+  </si>
+  <si>
+    <t>Pirate Grunt</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet01Template "Pirate Grunt" [NPC_:00010B2E]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet02 "Pirate Brigand" [NPC_:00010B38]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet03 "Pirate Freebooter" [NPC_:00009CED]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet04 "Pirate Rover" [NPC_:00009CEF]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet05 "Pirate Marauder" [NPC_:00009CEE]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet06 "Pirate Corsair" [NPC_:0012D034]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet07 "Pirate Plunderer" [NPC_:0012D033]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet08 "Pirate Reaver" [NPC_:0012D032]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet09 "Pirate Cutthroat" [NPC_:0012D031]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet10 "Pirate Flayer" [NPC_:0012D030]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet11 "Pirate Captain" [NPC_:0012D02F]</t>
+  </si>
+  <si>
+    <t>EncCrimsonFleet12 "Pirate Legend" [NPC_:0012D02E]</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1476,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1506,13 +1497,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1523,10 +1514,10 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D2" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -1541,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1555,7 +1546,7 @@
         <v>999</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
@@ -1573,10 +1564,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="K3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1587,7 +1578,7 @@
         <v>999</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
@@ -1605,10 +1596,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1619,7 +1610,7 @@
         <v>999</v>
       </c>
       <c r="C5" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -1637,10 +1628,10 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="K5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1651,7 +1642,7 @@
         <v>999</v>
       </c>
       <c r="C6" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -1669,234 +1660,234 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>213</v>
+      </c>
+      <c r="K7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>211</v>
+      </c>
+      <c r="K8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>125</v>
+      </c>
+      <c r="G9">
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>209</v>
+      </c>
+      <c r="K9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>125</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>220</v>
+      </c>
+      <c r="K10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>219</v>
       </c>
-      <c r="K6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="K11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>207</v>
+      </c>
+      <c r="K12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="K7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="1">
-        <v>100</v>
-      </c>
-      <c r="F8" s="1">
-        <v>100</v>
-      </c>
-      <c r="G8" s="1">
-        <v>50</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13">
         <v>150</v>
       </c>
-      <c r="F9" s="1">
-        <v>125</v>
-      </c>
-      <c r="G9" s="1">
-        <v>75</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="K9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="1">
-        <v>150</v>
-      </c>
-      <c r="F10" s="1">
-        <v>125</v>
-      </c>
-      <c r="G10" s="1">
-        <v>75</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="K10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>75</v>
-      </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="1">
-        <v>200</v>
-      </c>
-      <c r="F11" s="1">
-        <v>150</v>
-      </c>
-      <c r="G11" s="1">
-        <v>100</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>75</v>
-      </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1">
-        <v>200</v>
-      </c>
-      <c r="F12" s="1">
-        <v>150</v>
-      </c>
-      <c r="G12" s="1">
-        <v>100</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="K12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="1">
-        <v>300</v>
-      </c>
-      <c r="F13" s="1">
-        <v>200</v>
-      </c>
-      <c r="G13" s="1">
-        <v>150</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>1.05</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>221</v>
+      <c r="J13" t="s">
+        <v>205</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1907,7 +1898,7 @@
         <v>999</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
@@ -1925,10 +1916,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J14" t="s">
-        <v>234</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>320</v>
+        <v>218</v>
+      </c>
+      <c r="K14" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1939,10 +1930,10 @@
         <v>999</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -1957,10 +1948,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J16" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K16" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -1970,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BAB40E-ADE8-4D0F-8707-0DC6F2BA8471}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,18 +1972,17 @@
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2010,19 +2000,16 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
+      </c>
+      <c r="I1" t="s">
+        <v>187</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2030,10 +2017,10 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -2047,28 +2034,25 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="I2" t="s">
+        <v>309</v>
+      </c>
+      <c r="J2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>999</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>999</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -2082,28 +2066,25 @@
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>185</v>
-      </c>
-      <c r="L3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="I3" t="s">
+        <v>310</v>
+      </c>
+      <c r="J3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>999</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>999</v>
-      </c>
-      <c r="C4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -2117,28 +2098,25 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="K4" t="s">
-        <v>185</v>
-      </c>
-      <c r="L4" t="s">
-        <v>81</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="I4" t="s">
+        <v>311</v>
+      </c>
+      <c r="J4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>999</v>
-      </c>
-      <c r="C5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -2152,355 +2130,299 @@
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>185</v>
-      </c>
-      <c r="L5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="I5" t="s">
+        <v>312</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>999</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>999</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100</v>
+      </c>
+      <c r="G6" s="1">
+        <v>50</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <v>999</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E6">
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+      <c r="G7" s="1">
         <v>50</v>
       </c>
-      <c r="F6">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1">
+        <v>999</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="1">
+        <v>150</v>
+      </c>
+      <c r="F8" s="1">
+        <v>125</v>
+      </c>
+      <c r="G8" s="1">
+        <v>75</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1">
+        <v>999</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="1">
+        <v>150</v>
+      </c>
+      <c r="F9" s="1">
+        <v>125</v>
+      </c>
+      <c r="G9" s="1">
+        <v>75</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1">
+        <v>999</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="1">
+        <v>200</v>
+      </c>
+      <c r="F10" s="1">
+        <v>150</v>
+      </c>
+      <c r="G10" s="1">
+        <v>100</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>75</v>
+      </c>
+      <c r="B11" s="1">
+        <v>999</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="1">
+        <v>200</v>
+      </c>
+      <c r="F11" s="1">
+        <v>150</v>
+      </c>
+      <c r="G11" s="1">
+        <v>100</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>100</v>
+      </c>
+      <c r="B12" s="1">
+        <v>999</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="1">
+        <v>300</v>
+      </c>
+      <c r="F12" s="1">
+        <v>200</v>
+      </c>
+      <c r="G12" s="1">
+        <v>150</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.05</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>100</v>
+      </c>
+      <c r="B13" s="1">
+        <v>999</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="1">
+        <v>400</v>
+      </c>
+      <c r="F13" s="1">
+        <v>400</v>
+      </c>
+      <c r="G13" s="1">
+        <v>250</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="G15">
         <v>25</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>185</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>25</v>
-      </c>
-      <c r="B7">
-        <v>999</v>
-      </c>
-      <c r="C7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="G7">
-        <v>50</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>185</v>
-      </c>
-      <c r="L7" t="s">
-        <v>89</v>
-      </c>
-      <c r="M7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>999</v>
-      </c>
-      <c r="C8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="G8">
-        <v>50</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>185</v>
-      </c>
-      <c r="L8" t="s">
-        <v>91</v>
-      </c>
-      <c r="M8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>50</v>
-      </c>
-      <c r="B9">
-        <v>999</v>
-      </c>
-      <c r="C9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9">
-        <v>150</v>
-      </c>
-      <c r="F9">
-        <v>125</v>
-      </c>
-      <c r="G9">
-        <v>75</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>185</v>
-      </c>
-      <c r="L9" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>50</v>
-      </c>
-      <c r="B10">
-        <v>999</v>
-      </c>
-      <c r="C10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10">
-        <v>150</v>
-      </c>
-      <c r="F10">
-        <v>125</v>
-      </c>
-      <c r="G10">
-        <v>75</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>185</v>
-      </c>
-      <c r="L10" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>75</v>
-      </c>
-      <c r="B11">
-        <v>999</v>
-      </c>
-      <c r="C11" t="s">
-        <v>207</v>
-      </c>
-      <c r="D11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11">
-        <v>200</v>
-      </c>
-      <c r="F11">
-        <v>150</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>185</v>
-      </c>
-      <c r="L11" t="s">
-        <v>97</v>
-      </c>
-      <c r="M11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>75</v>
-      </c>
-      <c r="B12">
-        <v>999</v>
-      </c>
-      <c r="C12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12">
-        <v>150</v>
-      </c>
-      <c r="G12">
-        <v>100</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>185</v>
-      </c>
-      <c r="L12" t="s">
-        <v>99</v>
-      </c>
-      <c r="M12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>100</v>
-      </c>
-      <c r="B13">
-        <v>999</v>
-      </c>
-      <c r="C13" t="s">
-        <v>209</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13">
-        <v>300</v>
-      </c>
-      <c r="F13">
-        <v>200</v>
-      </c>
-      <c r="G13">
-        <v>150</v>
-      </c>
-      <c r="H13">
-        <v>1.05</v>
-      </c>
-      <c r="K13" t="s">
-        <v>185</v>
-      </c>
-      <c r="L13" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>100</v>
-      </c>
-      <c r="B14">
-        <v>999</v>
-      </c>
-      <c r="C14" t="s">
-        <v>210</v>
-      </c>
-      <c r="D14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E14">
-        <v>400</v>
-      </c>
-      <c r="F14">
-        <v>400</v>
-      </c>
-      <c r="G14">
-        <v>250</v>
-      </c>
-      <c r="H14">
+      <c r="H15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K14" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>999</v>
-      </c>
-      <c r="C16" t="s">
-        <v>186</v>
-      </c>
-      <c r="D16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16">
-        <v>50</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
-        <v>25</v>
-      </c>
-      <c r="H16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J16" t="s">
-        <v>193</v>
-      </c>
-      <c r="K16" t="s">
-        <v>321</v>
+      <c r="I15" t="s">
+        <v>190</v>
+      </c>
+      <c r="J15" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +2450,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2549,13 +2471,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2566,10 +2488,10 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -2587,7 +2509,7 @@
         <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2598,10 +2520,10 @@
         <v>999</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -2619,7 +2541,7 @@
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2630,10 +2552,10 @@
         <v>999</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -2651,7 +2573,7 @@
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2662,10 +2584,10 @@
         <v>999</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -2683,7 +2605,7 @@
         <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2694,10 +2616,10 @@
         <v>999</v>
       </c>
       <c r="C6" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -2715,263 +2637,263 @@
         <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>125</v>
+      </c>
+      <c r="G9">
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>125</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>235</v>
+      </c>
+      <c r="K10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>236</v>
+      </c>
+      <c r="K11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>237</v>
+      </c>
+      <c r="K12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13">
+        <v>150</v>
+      </c>
+      <c r="H13">
+        <v>1.05</v>
+      </c>
+      <c r="J13" t="s">
+        <v>238</v>
+      </c>
+      <c r="K13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="1">
-        <v>100</v>
-      </c>
-      <c r="F7" s="1">
-        <v>100</v>
-      </c>
-      <c r="G7" s="1">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="1">
-        <v>100</v>
-      </c>
-      <c r="F8" s="1">
-        <v>100</v>
-      </c>
-      <c r="G8" s="1">
-        <v>50</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="1">
-        <v>150</v>
-      </c>
-      <c r="F9" s="1">
-        <v>125</v>
-      </c>
-      <c r="G9" s="1">
-        <v>75</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="1">
-        <v>150</v>
-      </c>
-      <c r="F10" s="1">
-        <v>125</v>
-      </c>
-      <c r="G10" s="1">
-        <v>75</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>75</v>
-      </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="1">
-        <v>200</v>
-      </c>
-      <c r="F11" s="1">
-        <v>150</v>
-      </c>
-      <c r="G11" s="1">
-        <v>100</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="K11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>75</v>
-      </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" s="1">
-        <v>200</v>
-      </c>
-      <c r="F12" s="1">
-        <v>150</v>
-      </c>
-      <c r="G12" s="1">
-        <v>100</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="K12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="1">
-        <v>300</v>
-      </c>
-      <c r="F13" s="1">
-        <v>200</v>
-      </c>
-      <c r="G13" s="1">
-        <v>150</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="K13" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>100</v>
-      </c>
-      <c r="B14" s="1">
-        <v>999</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14">
+        <v>400</v>
+      </c>
+      <c r="F14">
+        <v>400</v>
+      </c>
+      <c r="G14">
         <v>250</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="1">
-        <v>400</v>
-      </c>
-      <c r="F14" s="1">
-        <v>400</v>
-      </c>
-      <c r="G14" s="1">
-        <v>250</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>255</v>
+      <c r="J14" t="s">
+        <v>239</v>
       </c>
       <c r="K14" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -2999,10 +2921,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3020,13 +2942,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3037,10 +2959,10 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -3055,10 +2977,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="K2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3069,10 +2991,10 @@
         <v>999</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3090,7 +3012,7 @@
         <v>7</v>
       </c>
       <c r="K3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3101,7 +3023,7 @@
         <v>999</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
@@ -3122,7 +3044,7 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3133,7 +3055,7 @@
         <v>999</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -3154,7 +3076,7 @@
         <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3165,7 +3087,7 @@
         <v>999</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D6" t="s">
         <v>39</v>
@@ -3186,263 +3108,263 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="K7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>25</v>
       </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>100</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>50</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="K8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>50</v>
       </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>150</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>125</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>75</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>258</v>
+      </c>
+      <c r="K9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>50</v>
       </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>150</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>125</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>75</v>
       </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="K10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>75</v>
       </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>200</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>150</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>257</v>
+      </c>
+      <c r="K11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>75</v>
       </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>200</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>150</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>256</v>
+      </c>
+      <c r="K12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>100</v>
       </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>300</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>200</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>150</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>1.05</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="J13" t="s">
+        <v>251</v>
+      </c>
+      <c r="K13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>100</v>
       </c>
-      <c r="B14" s="1">
-        <v>999</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="B14">
+        <v>999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>400</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>400</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>250</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>323</v>
+      <c r="J14" t="s">
+        <v>259</v>
+      </c>
+      <c r="K14" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3453,10 +3375,10 @@
         <v>999</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -3471,10 +3393,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K16" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3502,10 +3424,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3523,13 +3445,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3540,7 +3462,7 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
         <v>60</v>
@@ -3558,10 +3480,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="K2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3572,10 +3494,10 @@
         <v>999</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3590,10 +3512,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="K3" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3604,7 +3526,7 @@
         <v>999</v>
       </c>
       <c r="C4" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -3625,7 +3547,7 @@
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3636,7 +3558,7 @@
         <v>999</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
@@ -3657,7 +3579,7 @@
         <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3668,7 +3590,7 @@
         <v>999</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
@@ -3689,263 +3611,263 @@
         <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>282</v>
+      </c>
+      <c r="K8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9">
+        <v>150</v>
+      </c>
+      <c r="F9">
+        <v>125</v>
+      </c>
+      <c r="G9">
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>283</v>
+      </c>
+      <c r="K9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10">
+        <v>125</v>
+      </c>
+      <c r="G10">
+        <v>75</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>284</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="K10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>75</v>
+      </c>
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+      <c r="G11">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>285</v>
+      </c>
+      <c r="K11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>75</v>
+      </c>
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="K12" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>100</v>
       </c>
-      <c r="F8" s="1">
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>270</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13">
+        <v>150</v>
+      </c>
+      <c r="H13">
+        <v>1.05</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>100</v>
       </c>
-      <c r="G8" s="1">
-        <v>50</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" s="1">
-        <v>150</v>
-      </c>
-      <c r="F9" s="1">
-        <v>125</v>
-      </c>
-      <c r="G9" s="1">
-        <v>75</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="1">
-        <v>150</v>
-      </c>
-      <c r="F10" s="1">
-        <v>125</v>
-      </c>
-      <c r="G10" s="1">
-        <v>75</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>75</v>
-      </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="1">
-        <v>200</v>
-      </c>
-      <c r="F11" s="1">
-        <v>150</v>
-      </c>
-      <c r="G11" s="1">
-        <v>100</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>75</v>
-      </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="1">
-        <v>200</v>
-      </c>
-      <c r="F12" s="1">
-        <v>150</v>
-      </c>
-      <c r="G12" s="1">
-        <v>100</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="1">
-        <v>300</v>
-      </c>
-      <c r="F13" s="1">
-        <v>200</v>
-      </c>
-      <c r="G13" s="1">
-        <v>150</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1.05</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>100</v>
-      </c>
-      <c r="B14" s="1">
-        <v>999</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>287</v>
+      <c r="B14">
+        <v>999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>400</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>400</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>250</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>302</v>
+      <c r="J14" t="s">
+        <v>286</v>
       </c>
       <c r="K14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3956,10 +3878,10 @@
         <v>999</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -3974,10 +3896,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3988,10 +3910,10 @@
         <v>999</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E17">
         <v>5000</v>
@@ -4006,10 +3928,10 @@
         <v>1.25</v>
       </c>
       <c r="J17" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="K17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4021,7 +3943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB0993F-B9C8-4F81-89BA-D25D4095DD6F}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -4037,10 +3959,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4058,13 +3980,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -4075,7 +3997,7 @@
         <v>999</v>
       </c>
       <c r="C2" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -4093,10 +4015,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="K2" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4107,7 +4029,7 @@
         <v>999</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D3" t="s">
         <v>71</v>
@@ -4128,7 +4050,7 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4139,7 +4061,7 @@
         <v>999</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -4160,7 +4082,7 @@
         <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4171,7 +4093,7 @@
         <v>999</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
         <v>73</v>
@@ -4192,7 +4114,7 @@
         <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -4203,7 +4125,7 @@
         <v>999</v>
       </c>
       <c r="C6" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D6" t="s">
         <v>74</v>
@@ -4224,167 +4146,167 @@
         <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>318</v>
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>302</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>319</v>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>303</v>
       </c>
       <c r="K7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>50</v>
       </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>150</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>125</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>75</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>31</v>
       </c>
       <c r="K8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>75</v>
       </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>200</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>150</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>100</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
         <v>32</v>
       </c>
       <c r="K9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>100</v>
       </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>300</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>200</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>150</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
         <v>1.05</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>33</v>
       </c>
       <c r="K10" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>100</v>
       </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>315</v>
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>299</v>
       </c>
       <c r="D11" t="s">
-        <v>316</v>
-      </c>
-      <c r="E11" s="1">
+        <v>300</v>
+      </c>
+      <c r="E11">
         <v>400</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>400</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>250</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>317</v>
+      <c r="J11" t="s">
+        <v>301</v>
       </c>
       <c r="K11" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4432,7 +4354,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2">
         <f>FLOOR((0+(5*A2))*1.25, 1)</f>
@@ -4451,7 +4373,7 @@
         <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C3">
         <f>FLOOR((0+(5*A3))*1.25, 1)</f>
@@ -4470,7 +4392,7 @@
         <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C36" si="1">FLOOR((0+(5*A4))*1.25, 1)</f>
@@ -4489,7 +4411,7 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -4508,7 +4430,7 @@
         <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -4527,7 +4449,7 @@
         <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -4546,7 +4468,7 @@
         <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -4565,7 +4487,7 @@
         <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -4584,7 +4506,7 @@
         <v>165</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -4603,7 +4525,7 @@
         <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -4622,7 +4544,7 @@
         <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -4641,7 +4563,7 @@
         <v>180</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -4660,7 +4582,7 @@
         <v>185</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -4679,7 +4601,7 @@
         <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -4698,7 +4620,7 @@
         <v>195</v>
       </c>
       <c r="B16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -4717,7 +4639,7 @@
         <v>200</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -4736,7 +4658,7 @@
         <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -4755,7 +4677,7 @@
         <v>210</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
@@ -4774,7 +4696,7 @@
         <v>215</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
@@ -4793,7 +4715,7 @@
         <v>220</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
@@ -4812,7 +4734,7 @@
         <v>225</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
@@ -4831,7 +4753,7 @@
         <v>230</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4850,7 +4772,7 @@
         <v>235</v>
       </c>
       <c r="B24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4869,7 +4791,7 @@
         <v>240</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4888,7 +4810,7 @@
         <v>245</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4907,7 +4829,7 @@
         <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4926,7 +4848,7 @@
         <v>255</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4945,7 +4867,7 @@
         <v>260</v>
       </c>
       <c r="B29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4964,7 +4886,7 @@
         <v>265</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4983,7 +4905,7 @@
         <v>270</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -5002,7 +4924,7 @@
         <v>275</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -5021,7 +4943,7 @@
         <v>280</v>
       </c>
       <c r="B33" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -5040,7 +4962,7 @@
         <v>285</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -5059,7 +4981,7 @@
         <v>290</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -5078,7 +5000,7 @@
         <v>295</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -5097,7 +5019,7 @@
         <v>300</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C37">
         <v>2500</v>
@@ -5144,7 +5066,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -5153,7 +5075,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5166,7 +5088,7 @@
         <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3" si="0">FLOOR(500+((20*A3)*1.25), 1)</f>
@@ -5181,7 +5103,7 @@
       </c>
       <c r="H3">
         <f ca="1">H2+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>17.369999999999997</v>
+        <v>15.12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5189,7 +5111,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4" si="2">FLOOR(500+((20*A4)*1.25), 1)</f>
@@ -5204,7 +5126,7 @@
       </c>
       <c r="H4">
         <f ca="1">H3+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>21.119999999999997</v>
+        <v>15.87</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5212,7 +5134,7 @@
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5" si="3">FLOOR(500+((20*A5)*1.25), 1)</f>
@@ -5227,7 +5149,7 @@
       </c>
       <c r="H5">
         <f ca="1">H4+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>27.369999999999997</v>
+        <v>21.619999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5235,7 +5157,7 @@
         <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6" si="4">FLOOR(500+((20*A6)*1.25), 1)</f>
@@ -5250,7 +5172,7 @@
       </c>
       <c r="H6">
         <f ca="1">H5+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>29.619999999999997</v>
+        <v>26.869999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5258,7 +5180,7 @@
         <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C24" si="5">FLOOR(500+((20*A7)*1.25), 1)</f>
@@ -5273,7 +5195,7 @@
       </c>
       <c r="H7">
         <f ca="1">H6+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>34.119999999999997</v>
+        <v>32.369999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5281,7 +5203,7 @@
         <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C8">
         <f t="shared" si="5"/>
@@ -5296,7 +5218,7 @@
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H24" ca="1" si="6">H7+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>34.869999999999997</v>
+        <v>37.119999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5304,7 +5226,7 @@
         <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C9">
         <f t="shared" si="5"/>
@@ -5319,7 +5241,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>41.12</v>
+        <v>42.87</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5327,7 +5249,7 @@
         <v>160</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10">
         <f t="shared" si="5"/>
@@ -5342,7 +5264,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>43.37</v>
+        <v>45.87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5350,7 +5272,7 @@
         <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C11">
         <f t="shared" si="5"/>
@@ -5365,7 +5287,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="6"/>
-        <v>44.12</v>
+        <v>49.37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5373,7 +5295,7 @@
         <v>180</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C12">
         <f t="shared" si="5"/>
@@ -5388,7 +5310,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="6"/>
-        <v>48.12</v>
+        <v>54.87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5396,7 +5318,7 @@
         <v>190</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C13">
         <f t="shared" si="5"/>
@@ -5411,7 +5333,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="6"/>
-        <v>51.87</v>
+        <v>57.62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5419,7 +5341,7 @@
         <v>200</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C14">
         <f t="shared" si="5"/>
@@ -5434,7 +5356,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="6"/>
-        <v>53.87</v>
+        <v>57.87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5442,7 +5364,7 @@
         <v>210</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15">
         <f t="shared" si="5"/>
@@ -5457,7 +5379,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="6"/>
-        <v>56.12</v>
+        <v>58.87</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5465,7 +5387,7 @@
         <v>220</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C16">
         <f t="shared" si="5"/>
@@ -5480,7 +5402,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="6"/>
-        <v>62.12</v>
+        <v>62.37</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5488,7 +5410,7 @@
         <v>230</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C17">
         <f t="shared" si="5"/>
@@ -5503,7 +5425,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="6"/>
-        <v>64.62</v>
+        <v>67.62</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5511,7 +5433,7 @@
         <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C18">
         <f t="shared" si="5"/>
@@ -5526,7 +5448,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="6"/>
-        <v>70.62</v>
+        <v>72.87</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -5534,7 +5456,7 @@
         <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C19">
         <f t="shared" si="5"/>
@@ -5549,7 +5471,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="6"/>
-        <v>73.12</v>
+        <v>77.62</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5557,7 +5479,7 @@
         <v>260</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C20">
         <f t="shared" si="5"/>
@@ -5572,7 +5494,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="6"/>
-        <v>78.12</v>
+        <v>81.87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5580,7 +5502,7 @@
         <v>270</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C21">
         <f t="shared" si="5"/>
@@ -5595,7 +5517,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="6"/>
-        <v>81.37</v>
+        <v>85.12</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5603,7 +5525,7 @@
         <v>280</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C22">
         <f t="shared" si="5"/>
@@ -5618,7 +5540,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="6"/>
-        <v>84.87</v>
+        <v>88.37</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5626,7 +5548,7 @@
         <v>290</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C23">
         <f t="shared" si="5"/>
@@ -5641,7 +5563,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="6"/>
-        <v>87.62</v>
+        <v>88.87</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5649,7 +5571,7 @@
         <v>300</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C24">
         <f t="shared" si="5"/>
@@ -5664,7 +5586,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="6"/>
-        <v>92.62</v>
+        <v>94.62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5672,7 +5594,7 @@
         <v>666</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C27">
         <v>20000</v>

</xml_diff>

<commit_message>
Have to scale resists now too and use modav to do it setvalue doesn't work
</commit_message>
<xml_diff>
--- a/NPCScaling.xlsx
+++ b/NPCScaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Public\Starfield Mods\starfield-level-based-scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB60762-120A-4479-A924-A87BCEA8691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A308A-8612-43C3-B156-A01FB5FF3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
+    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="6" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
   </bookViews>
   <sheets>
     <sheet name="Spacers (Full DS)" sheetId="15" r:id="rId1"/>
@@ -1048,9 +1048,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1963,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BAB40E-ADE8-4D0F-8707-0DC6F2BA8471}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,259 +2136,259 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6" s="1">
-        <v>999</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6">
+        <v>999</v>
+      </c>
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>100</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>313</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>314</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>50</v>
       </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>150</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>125</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>75</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>315</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>50</v>
       </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>150</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>125</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>75</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>316</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>75</v>
       </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>200</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>150</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>317</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>75</v>
       </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>200</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>150</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>318</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>300</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>200</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>150</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
         <v>1.05</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>319</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>100</v>
       </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>400</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>400</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>250</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" t="s">
         <v>320</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4318,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61E54B1-4E1F-4F39-BC42-A63E31143326}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,7 +5102,7 @@
       </c>
       <c r="H3">
         <f ca="1">H2+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>15.12</v>
+        <v>16.369999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,7 +5125,7 @@
       </c>
       <c r="H4">
         <f ca="1">H3+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>15.87</v>
+        <v>22.619999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5149,7 +5148,7 @@
       </c>
       <c r="H5">
         <f ca="1">H4+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>21.619999999999997</v>
+        <v>27.619999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5172,7 +5171,7 @@
       </c>
       <c r="H6">
         <f ca="1">H5+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>26.869999999999997</v>
+        <v>32.619999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5195,7 +5194,7 @@
       </c>
       <c r="H7">
         <f ca="1">H6+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>32.369999999999997</v>
+        <v>35.119999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5218,7 +5217,7 @@
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H24" ca="1" si="6">H7+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>37.119999999999997</v>
+        <v>35.869999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,7 +5240,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>42.87</v>
+        <v>40.619999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5264,7 +5263,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>45.87</v>
+        <v>44.87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5287,7 +5286,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="6"/>
-        <v>49.37</v>
+        <v>46.12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5310,7 +5309,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="6"/>
-        <v>54.87</v>
+        <v>46.62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5333,7 +5332,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="6"/>
-        <v>57.62</v>
+        <v>47.12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5356,7 +5355,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="6"/>
-        <v>57.87</v>
+        <v>47.87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5379,7 +5378,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="6"/>
-        <v>58.87</v>
+        <v>51.62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5402,7 +5401,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="6"/>
-        <v>62.37</v>
+        <v>56.87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5425,7 +5424,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="6"/>
-        <v>67.62</v>
+        <v>58.12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5448,7 +5447,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="6"/>
-        <v>72.87</v>
+        <v>61.12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -5471,7 +5470,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="6"/>
-        <v>77.62</v>
+        <v>65.87</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5494,7 +5493,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="6"/>
-        <v>81.87</v>
+        <v>66.87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5517,7 +5516,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="6"/>
-        <v>85.12</v>
+        <v>71.87</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5540,7 +5539,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="6"/>
-        <v>88.37</v>
+        <v>75.87</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5563,7 +5562,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="6"/>
-        <v>88.87</v>
+        <v>76.37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5586,7 +5585,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="6"/>
-        <v>94.62</v>
+        <v>77.87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
V2.0.12 more dyn scaling script fun (#24)
* Have to scale resists now too and use modav to do it setvalue doesn't work

* Clean up
</commit_message>
<xml_diff>
--- a/NPCScaling.xlsx
+++ b/NPCScaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Public\Starfield Mods\starfield-level-based-scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB60762-120A-4479-A924-A87BCEA8691C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A308A-8612-43C3-B156-A01FB5FF3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
+    <workbookView xWindow="38280" yWindow="-285" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="6" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
   </bookViews>
   <sheets>
     <sheet name="Spacers (Full DS)" sheetId="15" r:id="rId1"/>
@@ -1048,9 +1048,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1963,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BAB40E-ADE8-4D0F-8707-0DC6F2BA8471}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,259 +2136,259 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6" s="1">
-        <v>999</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6">
+        <v>999</v>
+      </c>
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
         <v>100</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>313</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7" s="1">
-        <v>999</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7">
+        <v>999</v>
+      </c>
+      <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
         <v>100</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>314</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>50</v>
       </c>
-      <c r="B8" s="1">
-        <v>999</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8">
+        <v>999</v>
+      </c>
+      <c r="C8" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
         <v>150</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>125</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>75</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>315</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>50</v>
       </c>
-      <c r="B9" s="1">
-        <v>999</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9">
+        <v>999</v>
+      </c>
+      <c r="C9" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
         <v>150</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>125</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>75</v>
       </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>316</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>75</v>
       </c>
-      <c r="B10" s="1">
-        <v>999</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10">
+        <v>999</v>
+      </c>
+      <c r="C10" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>200</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>150</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>317</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>75</v>
       </c>
-      <c r="B11" s="1">
-        <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11">
+        <v>999</v>
+      </c>
+      <c r="C11" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>200</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>150</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>318</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>100</v>
       </c>
-      <c r="B12" s="1">
-        <v>999</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>300</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>200</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>150</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
         <v>1.05</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>319</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>100</v>
       </c>
-      <c r="B13" s="1">
-        <v>999</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13">
+        <v>999</v>
+      </c>
+      <c r="C13" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>400</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>400</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>250</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" t="s">
         <v>320</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4318,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61E54B1-4E1F-4F39-BC42-A63E31143326}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,7 +5102,7 @@
       </c>
       <c r="H3">
         <f ca="1">H2+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>15.12</v>
+        <v>16.369999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,7 +5125,7 @@
       </c>
       <c r="H4">
         <f ca="1">H3+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>15.87</v>
+        <v>22.619999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5149,7 +5148,7 @@
       </c>
       <c r="H5">
         <f ca="1">H4+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>21.619999999999997</v>
+        <v>27.619999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5172,7 +5171,7 @@
       </c>
       <c r="H6">
         <f ca="1">H5+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>26.869999999999997</v>
+        <v>32.619999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5195,7 +5194,7 @@
       </c>
       <c r="H7">
         <f ca="1">H6+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>32.369999999999997</v>
+        <v>35.119999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5218,7 +5217,7 @@
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H24" ca="1" si="6">H7+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>37.119999999999997</v>
+        <v>35.869999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,7 +5240,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>42.87</v>
+        <v>40.619999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5264,7 +5263,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>45.87</v>
+        <v>44.87</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5287,7 +5286,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="6"/>
-        <v>49.37</v>
+        <v>46.12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5310,7 +5309,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="6"/>
-        <v>54.87</v>
+        <v>46.62</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5333,7 +5332,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="6"/>
-        <v>57.62</v>
+        <v>47.12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5356,7 +5355,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="6"/>
-        <v>57.87</v>
+        <v>47.87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5379,7 +5378,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="6"/>
-        <v>58.87</v>
+        <v>51.62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5402,7 +5401,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="6"/>
-        <v>62.37</v>
+        <v>56.87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5425,7 +5424,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="6"/>
-        <v>67.62</v>
+        <v>58.12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5448,7 +5447,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="6"/>
-        <v>72.87</v>
+        <v>61.12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -5471,7 +5470,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="6"/>
-        <v>77.62</v>
+        <v>65.87</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5494,7 +5493,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="6"/>
-        <v>81.87</v>
+        <v>66.87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -5517,7 +5516,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="6"/>
-        <v>85.12</v>
+        <v>71.87</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5540,7 +5539,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="6"/>
-        <v>88.37</v>
+        <v>75.87</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5563,7 +5562,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="6"/>
-        <v>88.87</v>
+        <v>76.37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5586,7 +5585,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="6"/>
-        <v>94.62</v>
+        <v>77.87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Enabled scaling and cleanup debug messages
</commit_message>
<xml_diff>
--- a/NPCScaling.xlsx
+++ b/NPCScaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Public\Starfield Mods\starfield-level-based-scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22841498-48E8-4C3A-BE23-BAADDB4CBB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827F7B30-EFEE-4A1B-834B-E2E038668CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-240" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{3DA03D10-3AA7-4409-9B78-FCBABC3AD760}"/>
   </bookViews>
@@ -2185,6 +2185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2194,7 +2195,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -2739,13 +2739,13 @@
       <c r="I4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -2778,13 +2778,13 @@
       <c r="I5" t="s">
         <v>617</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -2818,13 +2818,13 @@
       <c r="I6" t="s">
         <v>619</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -5842,13 +5842,13 @@
       <c r="I4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -5881,13 +5881,13 @@
       <c r="I5" t="s">
         <v>624</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -5921,13 +5921,13 @@
       <c r="I6" t="s">
         <v>625</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -8941,13 +8941,13 @@
       <c r="I4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -8980,13 +8980,13 @@
       <c r="I5" t="s">
         <v>629</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -9020,13 +9020,13 @@
       <c r="I6" t="s">
         <v>630</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -11911,7 +11911,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11924,25 +11924,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>616</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>163</v>
       </c>
     </row>
@@ -12017,13 +12017,13 @@
       <c r="H4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -12050,13 +12050,13 @@
       <c r="H5" t="s">
         <v>640</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>642</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -12083,13 +12083,13 @@
       <c r="H6" t="s">
         <v>641</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -14490,7 +14490,7 @@
       </c>
       <c r="H3">
         <f ca="1">H2+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>14.37</v>
+        <v>13.37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -14513,7 +14513,7 @@
       </c>
       <c r="H4">
         <f ca="1">H3+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>20.119999999999997</v>
+        <v>15.87</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -14536,7 +14536,7 @@
       </c>
       <c r="H5">
         <f ca="1">H4+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>23.369999999999997</v>
+        <v>16.869999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -14559,7 +14559,7 @@
       </c>
       <c r="H6">
         <f ca="1">H5+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>26.369999999999997</v>
+        <v>19.619999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -14582,7 +14582,7 @@
       </c>
       <c r="H7">
         <f ca="1">H6+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>32.119999999999997</v>
+        <v>20.619999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -14605,7 +14605,7 @@
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H24" ca="1" si="6">H7+(RANDBETWEEN(1,25)*0.25)</f>
-        <v>37.869999999999997</v>
+        <v>26.619999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -14628,7 +14628,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>40.619999999999997</v>
+        <v>32.619999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -14651,7 +14651,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>46.37</v>
+        <v>37.619999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -14674,7 +14674,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="6"/>
-        <v>47.62</v>
+        <v>39.119999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -14697,7 +14697,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="6"/>
-        <v>51.37</v>
+        <v>44.12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -14720,7 +14720,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="6"/>
-        <v>54.12</v>
+        <v>50.37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -14743,7 +14743,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="6"/>
-        <v>60.37</v>
+        <v>52.37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -14766,7 +14766,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="6"/>
-        <v>65.62</v>
+        <v>57.37</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -14789,7 +14789,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="6"/>
-        <v>65.87</v>
+        <v>58.62</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -14812,7 +14812,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="6"/>
-        <v>68.62</v>
+        <v>62.12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -14835,7 +14835,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="6"/>
-        <v>74.37</v>
+        <v>66.12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -14858,7 +14858,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="6"/>
-        <v>78.62</v>
+        <v>70.37</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -14881,7 +14881,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="6"/>
-        <v>79.37</v>
+        <v>74.62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -14904,7 +14904,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="6"/>
-        <v>83.62</v>
+        <v>80.12</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -14927,7 +14927,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="6"/>
-        <v>85.37</v>
+        <v>81.37</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -14950,7 +14950,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="6"/>
-        <v>87.37</v>
+        <v>87.62</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -14973,7 +14973,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="6"/>
-        <v>92.37</v>
+        <v>90.87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>